<commit_message>
vocab updated w/ abs 2
</commit_message>
<xml_diff>
--- a/vocab_schulz_griesbach.xlsx
+++ b/vocab_schulz_griesbach.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Language\Deutsch\Schulz_Griesbach\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Language\Deutsch\Schulz_Griesbach_repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1018CA1A-496A-472B-86D4-8C5FD0CDB4D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162CC112-A5B0-404B-A52B-CBF28E766167}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="218">
   <si>
     <t>Abschnitt eins</t>
   </si>
@@ -349,6 +349,336 @@
   </si>
   <si>
     <t>Abschnitt zwei</t>
+  </si>
+  <si>
+    <t>der Unterricht</t>
+  </si>
+  <si>
+    <t>lesson</t>
+  </si>
+  <si>
+    <t>die Klasse</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>das Zimmer</t>
+  </si>
+  <si>
+    <t>room</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+e </t>
+  </si>
+  <si>
+    <t>beginnen</t>
+  </si>
+  <si>
+    <t>to begin</t>
+  </si>
+  <si>
+    <t>Guten Morgen!</t>
+  </si>
+  <si>
+    <t>good morning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jetzt </t>
+  </si>
+  <si>
+    <t>now</t>
+  </si>
+  <si>
+    <t>der Satz</t>
+  </si>
+  <si>
+    <t>ä, +e</t>
+  </si>
+  <si>
+    <t>sentence</t>
+  </si>
+  <si>
+    <t>wiederholen</t>
+  </si>
+  <si>
+    <t>to repeat</t>
+  </si>
+  <si>
+    <t>das Schulzimmer</t>
+  </si>
+  <si>
+    <t>classroom</t>
+  </si>
+  <si>
+    <t>der Fußboden</t>
+  </si>
+  <si>
+    <t>ö</t>
+  </si>
+  <si>
+    <t>floor</t>
+  </si>
+  <si>
+    <t>die Decke</t>
+  </si>
+  <si>
+    <t>ceiling</t>
+  </si>
+  <si>
+    <t>die Wand</t>
+  </si>
+  <si>
+    <t>wall</t>
+  </si>
+  <si>
+    <t>hängen</t>
+  </si>
+  <si>
+    <t>to hang</t>
+  </si>
+  <si>
+    <t>to be hanging</t>
+  </si>
+  <si>
+    <t>vorn</t>
+  </si>
+  <si>
+    <t>front</t>
+  </si>
+  <si>
+    <t>hier vorn</t>
+  </si>
+  <si>
+    <t>up front</t>
+  </si>
+  <si>
+    <t>hier oben</t>
+  </si>
+  <si>
+    <t>up here</t>
+  </si>
+  <si>
+    <t>hinten</t>
+  </si>
+  <si>
+    <t>behind</t>
+  </si>
+  <si>
+    <t>dort hinten</t>
+  </si>
+  <si>
+    <t>over there</t>
+  </si>
+  <si>
+    <t>Rechts</t>
+  </si>
+  <si>
+    <t>on the right</t>
+  </si>
+  <si>
+    <t>Links</t>
+  </si>
+  <si>
+    <t>on the left</t>
+  </si>
+  <si>
+    <t>die Tafel</t>
+  </si>
+  <si>
+    <t>board</t>
+  </si>
+  <si>
+    <t>die Kreide</t>
+  </si>
+  <si>
+    <t>chalk/crayon</t>
+  </si>
+  <si>
+    <t>der Schwamm</t>
+  </si>
+  <si>
+    <t>sponge</t>
+  </si>
+  <si>
+    <t>die Landkarte</t>
+  </si>
+  <si>
+    <t>map</t>
+  </si>
+  <si>
+    <t>die Tür</t>
+  </si>
+  <si>
+    <t>door</t>
+  </si>
+  <si>
+    <t>das Fenster</t>
+  </si>
+  <si>
+    <t>window</t>
+  </si>
+  <si>
+    <t>die Lampe</t>
+  </si>
+  <si>
+    <t>lamp</t>
+  </si>
+  <si>
+    <t>verbessern</t>
+  </si>
+  <si>
+    <t>to correct</t>
+  </si>
+  <si>
+    <t>der Fehler</t>
+  </si>
+  <si>
+    <t>mistake</t>
+  </si>
+  <si>
+    <t>sehr</t>
+  </si>
+  <si>
+    <t>very</t>
+  </si>
+  <si>
+    <t>zeigen</t>
+  </si>
+  <si>
+    <t>to show</t>
+  </si>
+  <si>
+    <t>heißen</t>
+  </si>
+  <si>
+    <t>to call</t>
+  </si>
+  <si>
+    <t>machen</t>
+  </si>
+  <si>
+    <t>to make/to do</t>
+  </si>
+  <si>
+    <t>bilden</t>
+  </si>
+  <si>
+    <t>to build</t>
+  </si>
+  <si>
+    <t>lang</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>kurz</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>klein</t>
+  </si>
+  <si>
+    <t>small</t>
+  </si>
+  <si>
+    <t>large</t>
+  </si>
+  <si>
+    <t>groß</t>
+  </si>
+  <si>
+    <t>das Gegenteil</t>
+  </si>
+  <si>
+    <t>opposite/contrary</t>
+  </si>
+  <si>
+    <t>diktieren</t>
+  </si>
+  <si>
+    <t>to dictate</t>
+  </si>
+  <si>
+    <t>schreiben</t>
+  </si>
+  <si>
+    <t>to write</t>
+  </si>
+  <si>
+    <t>erklären</t>
+  </si>
+  <si>
+    <t>to explain</t>
+  </si>
+  <si>
+    <t>verstehen</t>
+  </si>
+  <si>
+    <t>to understand</t>
+  </si>
+  <si>
+    <t>sondern</t>
+  </si>
+  <si>
+    <t>instead</t>
+  </si>
+  <si>
+    <t>das Kind</t>
+  </si>
+  <si>
+    <t>+er</t>
+  </si>
+  <si>
+    <t>kid</t>
+  </si>
+  <si>
+    <t>das Wort</t>
+  </si>
+  <si>
+    <t>ö, +er</t>
+  </si>
+  <si>
+    <t>word</t>
+  </si>
+  <si>
+    <t>die Stunde</t>
+  </si>
+  <si>
+    <t>hour</t>
+  </si>
+  <si>
+    <t>die Minute</t>
+  </si>
+  <si>
+    <t>minute</t>
+  </si>
+  <si>
+    <t>die Sekund</t>
+  </si>
+  <si>
+    <t>second</t>
+  </si>
+  <si>
+    <t>dauern</t>
+  </si>
+  <si>
+    <t>to last</t>
+  </si>
+  <si>
+    <t>ist aus</t>
+  </si>
+  <si>
+    <t>is over</t>
+  </si>
+  <si>
+    <t>schleißen</t>
+  </si>
+  <si>
+    <t>to close</t>
   </si>
 </sst>
 </file>
@@ -717,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -730,7 +1060,7 @@
     <col min="3" max="3" width="9.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="12.21875" style="7" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" customWidth="1"/>
     <col min="8" max="8" width="12.109375" style="8" customWidth="1"/>
     <col min="9" max="9" width="13" style="5" customWidth="1"/>
@@ -1128,7 +1458,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F17" t="s">
         <v>90</v>
       </c>
@@ -1139,7 +1469,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F18" t="s">
         <v>91</v>
       </c>
@@ -1150,7 +1480,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F19" t="s">
         <v>94</v>
       </c>
@@ -1161,7 +1491,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F20" t="s">
         <v>95</v>
       </c>
@@ -1172,7 +1502,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F21" t="s">
         <v>99</v>
       </c>
@@ -1183,7 +1513,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F22" t="s">
         <v>101</v>
       </c>
@@ -1194,7 +1524,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F23" t="s">
         <v>103</v>
       </c>
@@ -1205,7 +1535,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F24" t="s">
         <v>105</v>
       </c>
@@ -1216,9 +1546,488 @@
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>115</v>
+      </c>
+      <c r="B28" t="s">
+        <v>116</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" t="s">
+        <v>108</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="K28" t="s">
+        <v>180</v>
+      </c>
+      <c r="L28" t="s">
+        <v>181</v>
+      </c>
+      <c r="N28" t="s">
+        <v>14</v>
+      </c>
+      <c r="O28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>124</v>
+      </c>
+      <c r="B29" t="s">
+        <v>125</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" t="s">
+        <v>110</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="K29" t="s">
+        <v>182</v>
+      </c>
+      <c r="L29" t="s">
+        <v>183</v>
+      </c>
+      <c r="N29" t="s">
+        <v>117</v>
+      </c>
+      <c r="O29" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>135</v>
+      </c>
+      <c r="B30" t="s">
+        <v>136</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" t="s">
+        <v>112</v>
+      </c>
+      <c r="G30" t="s">
+        <v>52</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="K30" t="s">
+        <v>184</v>
+      </c>
+      <c r="L30" t="s">
+        <v>185</v>
+      </c>
+      <c r="N30" t="s">
+        <v>119</v>
+      </c>
+      <c r="O30" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>137</v>
+      </c>
+      <c r="F31" t="s">
+        <v>121</v>
+      </c>
+      <c r="G31" t="s">
+        <v>122</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="K31" t="s">
+        <v>187</v>
+      </c>
+      <c r="L31" t="s">
+        <v>186</v>
+      </c>
+      <c r="N31" t="s">
+        <v>138</v>
+      </c>
+      <c r="O31" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>166</v>
+      </c>
+      <c r="B32" t="s">
+        <v>167</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F32" t="s">
+        <v>126</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="N32" t="s">
+        <v>140</v>
+      </c>
+      <c r="O32" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>172</v>
+      </c>
+      <c r="B33" t="s">
+        <v>173</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" t="s">
+        <v>128</v>
+      </c>
+      <c r="G33" t="s">
+        <v>129</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="N33" t="s">
+        <v>142</v>
+      </c>
+      <c r="O33" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>174</v>
+      </c>
+      <c r="B34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" t="s">
+        <v>131</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="N34" t="s">
+        <v>144</v>
+      </c>
+      <c r="O34" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>176</v>
+      </c>
+      <c r="B35" t="s">
+        <v>177</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" t="s">
+        <v>133</v>
+      </c>
+      <c r="G35" t="s">
+        <v>122</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="N35" t="s">
+        <v>146</v>
+      </c>
+      <c r="O35" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>178</v>
+      </c>
+      <c r="B36" t="s">
+        <v>179</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" t="s">
+        <v>152</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="N36" t="s">
+        <v>148</v>
+      </c>
+      <c r="O36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>190</v>
+      </c>
+      <c r="B37" t="s">
+        <v>191</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" t="s">
+        <v>154</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="N37" t="s">
+        <v>150</v>
+      </c>
+      <c r="O37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>192</v>
+      </c>
+      <c r="B38" t="s">
+        <v>193</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" t="s">
+        <v>156</v>
+      </c>
+      <c r="G38" t="s">
+        <v>122</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="N38" t="s">
+        <v>170</v>
+      </c>
+      <c r="O38" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>194</v>
+      </c>
+      <c r="B39" t="s">
+        <v>195</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" t="s">
+        <v>158</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="N39" t="s">
+        <v>198</v>
+      </c>
+      <c r="O39" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>196</v>
+      </c>
+      <c r="B40" t="s">
+        <v>197</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" t="s">
+        <v>160</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="N40" t="s">
+        <v>214</v>
+      </c>
+      <c r="O40" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" t="s">
+        <v>162</v>
+      </c>
+      <c r="G41" t="s">
+        <v>52</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>212</v>
+      </c>
+      <c r="B42" t="s">
+        <v>213</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F42" t="s">
+        <v>164</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>216</v>
+      </c>
+      <c r="B43" t="s">
+        <v>217</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" t="s">
+        <v>168</v>
+      </c>
+      <c r="G43" t="s">
+        <v>52</v>
+      </c>
+      <c r="H43" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="F44" t="s">
+        <v>188</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H44" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="F45" t="s">
+        <v>200</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="H45" s="8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="F46" t="s">
+        <v>203</v>
+      </c>
+      <c r="G46" t="s">
+        <v>204</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="F47" t="s">
+        <v>206</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H47" s="8" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="F48" t="s">
+        <v>208</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H48" s="8" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="49" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F49" t="s">
+        <v>210</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H49" s="8" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>